<commit_message>
Vreg and ESD suppresion
</commit_message>
<xml_diff>
--- a/Jämförelse Komponenter.xlsx
+++ b/Jämförelse Komponenter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theozor\Documents\LuftIOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2771EB2-0346-4294-9643-BFAB4A5F5990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4545409A-33E3-4227-BC04-E199120E9565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="2565" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Lufttryck</t>
   </si>
@@ -80,9 +80,6 @@
     <t>BME688</t>
   </si>
   <si>
-    <t>BMP280</t>
-  </si>
-  <si>
     <t>SCD41-D-R2</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>400-10000 ppm, Stäng av autocalibrate</t>
   </si>
   <si>
-    <t>400-2000 ppm, Stäng av autocalibrate</t>
-  </si>
-  <si>
     <t>TVOC</t>
   </si>
   <si>
@@ -114,6 +108,9 @@
   </si>
   <si>
     <t>Kan mäta temp och är uppgradering av BME280. Tempmätning ogiltigt vid mätning av VOC</t>
+  </si>
+  <si>
+    <t>400-5000 ppm, Stäng av autocalibrate</t>
   </si>
 </sst>
 </file>
@@ -121,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -161,7 +158,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E9:V31"/>
+  <dimension ref="E9:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,14 +558,14 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P10" t="str">
         <f>IF(G10,$E10,"")</f>
         <v/>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" ref="Q10:V25" si="0">IF(H10,$E10,"")</f>
+        <f t="shared" ref="Q10:V24" si="0">IF(H10,$E10,"")</f>
         <v>LPS27HHWTR</v>
       </c>
       <c r="R10" t="str">
@@ -621,10 +618,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" ref="P11:P31" si="1">IF(G11,$E11,"")</f>
+        <f t="shared" ref="P11:P30" si="1">IF(G11,$E11,"")</f>
         <v/>
       </c>
       <c r="Q11" t="str">
@@ -681,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="1"/>
@@ -741,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="1"/>
@@ -774,10 +771,10 @@
     </row>
     <row r="14" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F14" s="2">
-        <v>2.9157000000000002</v>
+        <v>3.7465000000000002</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
@@ -789,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="1" t="b">
         <v>0</v>
@@ -800,13 +797,16 @@
       <c r="M14" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
       <c r="P14" t="str">
         <f t="shared" si="1"/>
-        <v>BMP280</v>
+        <v>BME280</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="0"/>
-        <v>BMP280</v>
+        <v>BME280</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="0"/>
@@ -814,7 +814,7 @@
       </c>
       <c r="S14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>BME280</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="0"/>
@@ -831,25 +831,25 @@
     </row>
     <row r="15" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2">
-        <v>3.7465000000000002</v>
+        <v>30.135000000000002</v>
       </c>
       <c r="G15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="H15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="b">
-        <v>0</v>
       </c>
       <c r="L15" s="1" t="b">
         <v>0</v>
@@ -862,11 +862,11 @@
       </c>
       <c r="P15" t="str">
         <f t="shared" si="1"/>
-        <v>BME280</v>
+        <v/>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="0"/>
-        <v>BME280</v>
+        <v/>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="0"/>
@@ -874,11 +874,11 @@
       </c>
       <c r="S15" t="str">
         <f t="shared" si="0"/>
-        <v>BME280</v>
+        <v/>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>SCD41-D-R2</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="0"/>
@@ -891,10 +891,10 @@
     </row>
     <row r="16" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2">
-        <v>30.135000000000002</v>
+        <v>51.5154</v>
       </c>
       <c r="G16" s="1" t="b">
         <v>0</v>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="1"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="T16" t="str">
         <f t="shared" si="0"/>
-        <v>SCD41-D-R2</v>
+        <v>SCD30</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="0"/>
@@ -951,10 +951,10 @@
     </row>
     <row r="17" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2">
-        <v>51.5154</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>0</v>
@@ -963,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1" t="b">
         <v>0</v>
@@ -977,9 +977,6 @@
       <c r="M17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="N17" t="s">
-        <v>20</v>
-      </c>
       <c r="P17" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -990,7 +987,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>PMS5003</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="0"/>
@@ -998,7 +995,7 @@
       </c>
       <c r="T17" t="str">
         <f t="shared" si="0"/>
-        <v>SCD30</v>
+        <v/>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="0"/>
@@ -1010,33 +1007,7 @@
       </c>
     </row>
     <row r="18" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="2">
-        <v>40</v>
-      </c>
-      <c r="G18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="P18" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1047,7 +1018,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" si="0"/>
-        <v>PMS5003</v>
+        <v/>
       </c>
       <c r="S18" t="str">
         <f t="shared" si="0"/>
@@ -1259,27 +1230,27 @@
         <v/>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q25:Q30" si="2">IF(H25,$E25,"")</f>
         <v/>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="R25:R30" si="3">IF(I25,$E25,"")</f>
         <v/>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S25:S30" si="4">IF(J25,$E25,"")</f>
         <v/>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="T25:T30" si="5">IF(K25,$E25,"")</f>
         <v/>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="U25:U30" si="6">IF(L25,$E25,"")</f>
         <v/>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="V25:V30" si="7">IF(M25,$E25,"")</f>
         <v/>
       </c>
     </row>
@@ -1290,27 +1261,27 @@
         <v/>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q26:Q31" si="2">IF(H26,$E26,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R26" t="str">
-        <f t="shared" ref="R26:R31" si="3">IF(I26,$E26,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S26" t="str">
-        <f t="shared" ref="S26:S31" si="4">IF(J26,$E26,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="T26" t="str">
-        <f t="shared" ref="T26:T31" si="5">IF(K26,$E26,"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="U26" t="str">
-        <f t="shared" ref="U26:U31" si="6">IF(L26,$E26,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="V26" t="str">
-        <f t="shared" ref="V26:V31" si="7">IF(M26,$E26,"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -1434,37 +1405,6 @@
         <v/>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="F31" s="2"/>
-      <c r="P31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q31" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="R31" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S31" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="T31" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="U31" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>

</xml_diff>